<commit_message>
20170914T2345 - Corrections agreed with e-Sens.
</commit_message>
<xml_diff>
--- a/docs/target/generated-docs/dist/cl/xlsx/ESPD-CodeLists-V02.00.00.xlsx
+++ b/docs/target/generated-docs/dist/cl/xlsx/ESPD-CodeLists-V02.00.00.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="7275" yWindow="1575" windowWidth="12630" windowHeight="6420" tabRatio="884" firstSheet="16" activeTab="23"/>
+    <workbookView xWindow="7275" yWindow="1575" windowWidth="12630" windowHeight="6420" tabRatio="884" firstSheet="5" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="ActivityType" sheetId="155" r:id="rId1"/>
@@ -4481,12 +4481,6 @@
     <t>CRITERION ELEMENT TYPE</t>
   </si>
   <si>
-    <t>Criterion</t>
-  </si>
-  <si>
-    <t>Question or requirement that requires an answer</t>
-  </si>
-  <si>
     <t>URL</t>
   </si>
   <si>
@@ -4613,33 +4607,12 @@
     <t>SUBCRITERION</t>
   </si>
   <si>
-    <t>Use to define national subcriteria or to group complex repetitive structures (e.g. more than one ratio or more than one references to works, supplies or services)</t>
-  </si>
-  <si>
-    <t>Group of requirements or remarks (captions)</t>
-  </si>
-  <si>
-    <t>Requirement, remark, additional information (captions)</t>
-  </si>
-  <si>
-    <t>Group of questions, each question requiring an answer</t>
-  </si>
-  <si>
     <t>QUESTION_SUBGROUP</t>
   </si>
   <si>
-    <t>A subgroup of questions inside a group or a subgroup of question</t>
-  </si>
-  <si>
-    <t>A subgroup of requirements or remarks (captions) inside a group or subgroup of requirements</t>
-  </si>
-  <si>
     <t>CAPTION</t>
   </si>
   <si>
-    <t>A text label</t>
-  </si>
-  <si>
     <t>Additional line in a description (for descriptions that can be split in several lines)</t>
   </si>
   <si>
@@ -5082,6 +5055,33 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>A criterion (in the case of the the ESPD an Exclusion or Selection criterion)</t>
+  </si>
+  <si>
+    <t>Used to define national sub-criteria</t>
+  </si>
+  <si>
+    <t>Group of requirements or remarks issued by a MS or a CA</t>
+  </si>
+  <si>
+    <t>A subgroup of requirements or remarks inside a group or subgroup of requirements</t>
+  </si>
+  <si>
+    <t>Requirement, remark, rule, restriction or additional information to which the EO needs to conform or comply with</t>
+  </si>
+  <si>
+    <t>Group of questions, each question requiring a datum as an answer from the EO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A subgroup of questions inside a group or a subgroup of questions</t>
+  </si>
+  <si>
+    <t>A question that requires an answer (a specific datum) from the EO</t>
+  </si>
+  <si>
+    <t>A text label (no requirement nor answer is expected)</t>
   </si>
 </sst>
 </file>
@@ -7931,7 +7931,7 @@
         <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>1599</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -8169,7 +8169,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>1454</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -8223,7 +8223,7 @@
         <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>1599</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -8293,7 +8293,7 @@
         <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1587</v>
+        <v>1578</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -8301,7 +8301,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1588</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -8309,7 +8309,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1587</v>
+        <v>1578</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -8317,7 +8317,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>1454</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -8371,47 +8371,47 @@
         <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>1599</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>1589</v>
+        <v>1580</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>1593</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>1590</v>
+        <v>1581</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>1594</v>
+        <v>1585</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>1591</v>
+        <v>1582</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>1595</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
-        <v>1597</v>
+        <v>1588</v>
       </c>
       <c r="B16" s="44" t="s">
-        <v>1598</v>
+        <v>1589</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>1592</v>
+        <v>1583</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>1596</v>
+        <v>1587</v>
       </c>
     </row>
   </sheetData>
@@ -8468,7 +8468,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>1454</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -8522,7 +8522,7 @@
         <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>1599</v>
+        <v>1590</v>
       </c>
       <c r="C12" t="s">
         <v>1187</v>
@@ -8671,7 +8671,7 @@
         <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>1599</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -8971,7 +8971,7 @@
         <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>1599</v>
+        <v>1590</v>
       </c>
       <c r="C12" t="s">
         <v>1317</v>
@@ -9347,7 +9347,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>1454</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -9401,7 +9401,7 @@
         <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>1599</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -9471,7 +9471,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>1454</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -9525,7 +9525,7 @@
         <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>1599</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -9618,7 +9618,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>1454</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -9672,7 +9672,7 @@
         <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>1599</v>
+        <v>1590</v>
       </c>
       <c r="C12" t="s">
         <v>1277</v>
@@ -9761,7 +9761,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>1454</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -9815,7 +9815,7 @@
         <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>1599</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -9939,7 +9939,7 @@
         <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>1599</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -10114,7 +10114,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>1454</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -10168,7 +10168,7 @@
         <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>1599</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -10397,7 +10397,7 @@
         <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>1599</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -10538,7 +10538,7 @@
         <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>1599</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -10624,7 +10624,7 @@
         <v>26</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>1576</v>
+        <v>1567</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -10638,7 +10638,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>1577</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -10646,7 +10646,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>1454</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -10704,31 +10704,31 @@
         <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>1599</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="37" t="s">
-        <v>1578</v>
+        <v>1569</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>1581</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="37" t="s">
-        <v>1579</v>
+        <v>1570</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>1582</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="37" t="s">
-        <v>1580</v>
+        <v>1571</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>1583</v>
+        <v>1574</v>
       </c>
     </row>
   </sheetData>
@@ -10784,7 +10784,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="42" t="s">
-        <v>1454</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -10842,7 +10842,7 @@
         <v>30</v>
       </c>
       <c r="B12" s="40" t="s">
-        <v>1599</v>
+        <v>1590</v>
       </c>
       <c r="C12" s="40" t="s">
         <v>1187</v>
@@ -10883,7 +10883,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -10922,7 +10922,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>1454</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -10976,7 +10976,7 @@
         <v>30</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>1599</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -11021,10 +11021,10 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
-        <v>1585</v>
+        <v>1576</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>1586</v>
+        <v>1577</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -11088,79 +11088,79 @@
         <v>1313</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>1584</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
-        <v>1401</v>
+        <v>1399</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>1402</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="23" t="s">
-        <v>1425</v>
+        <v>1423</v>
       </c>
       <c r="B28" s="31" t="s">
-        <v>1437</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="23" t="s">
-        <v>1426</v>
+        <v>1424</v>
       </c>
       <c r="B29" s="31" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="23" t="s">
-        <v>1427</v>
+        <v>1425</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>1436</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="23" t="s">
-        <v>1428</v>
+        <v>1426</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>1435</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="23" t="s">
-        <v>1429</v>
+        <v>1427</v>
       </c>
       <c r="B32" s="23" t="s">
-        <v>1434</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="23" t="s">
+        <v>1428</v>
+      </c>
+      <c r="B33" s="23" t="s">
         <v>1430</v>
-      </c>
-      <c r="B33" s="23" t="s">
-        <v>1432</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="23" t="s">
+        <v>1429</v>
+      </c>
+      <c r="B34" s="23" t="s">
         <v>1431</v>
-      </c>
-      <c r="B34" s="23" t="s">
-        <v>1433</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="23" t="s">
-        <v>1439</v>
+        <v>1437</v>
       </c>
       <c r="B35" s="23" t="s">
-        <v>1440</v>
+        <v>1438</v>
       </c>
     </row>
   </sheetData>
@@ -11267,7 +11267,7 @@
         <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>1599</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -11592,7 +11592,7 @@
         <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>1599</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -11827,7 +11827,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>1454</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -11881,7 +11881,7 @@
         <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>1599</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -12002,7 +12002,7 @@
         <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>1599</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -12178,7 +12178,7 @@
         <v>30</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>1599</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
@@ -14190,8 +14190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14229,7 +14229,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>1454</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -14283,7 +14283,7 @@
         <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>1599</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -14291,87 +14291,87 @@
         <v>1396</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>1399</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
-        <v>1442</v>
+        <v>1440</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>1443</v>
+        <v>1592</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
-        <v>1421</v>
+        <v>1419</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>1444</v>
+        <v>1593</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
-        <v>1441</v>
+        <v>1439</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>1449</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
-        <v>1422</v>
+        <v>1420</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>1445</v>
+        <v>1595</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
-        <v>1423</v>
+        <v>1421</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>1446</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
-        <v>1447</v>
+        <v>1441</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>1448</v>
+        <v>1597</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
-        <v>1424</v>
+        <v>1422</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>1400</v>
+        <v>1598</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
-        <v>1450</v>
+        <v>1442</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>1451</v>
+        <v>1599</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
-        <v>1453</v>
+        <v>1444</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>1452</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
-        <v>1455</v>
+        <v>1446</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>1456</v>
+        <v>1447</v>
       </c>
     </row>
   </sheetData>
@@ -14428,7 +14428,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1454</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -14482,7 +14482,7 @@
         <v>30</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>1457</v>
+        <v>1448</v>
       </c>
       <c r="C12" s="33" t="s">
         <v>1187</v>
@@ -14493,13 +14493,13 @@
         <v>1194</v>
       </c>
       <c r="B13" s="35" t="s">
-        <v>1458</v>
+        <v>1449</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>1459</v>
+        <v>1450</v>
       </c>
       <c r="D13" s="35" t="s">
-        <v>1460</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -14507,13 +14507,13 @@
         <v>1195</v>
       </c>
       <c r="B14" s="35" t="s">
-        <v>1461</v>
+        <v>1452</v>
       </c>
       <c r="C14" s="35" t="s">
-        <v>1462</v>
+        <v>1453</v>
       </c>
       <c r="D14" s="35" t="s">
-        <v>1460</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -14521,10 +14521,10 @@
         <v>1196</v>
       </c>
       <c r="B15" s="35" t="s">
-        <v>1463</v>
+        <v>1454</v>
       </c>
       <c r="D15" s="35" t="s">
-        <v>1460</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -14532,13 +14532,13 @@
         <v>1197</v>
       </c>
       <c r="B16" s="35" t="s">
-        <v>1464</v>
+        <v>1455</v>
       </c>
       <c r="C16" s="35" t="s">
-        <v>1465</v>
+        <v>1456</v>
       </c>
       <c r="D16" s="35" t="s">
-        <v>1460</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -14546,10 +14546,10 @@
         <v>1198</v>
       </c>
       <c r="B17" s="35" t="s">
-        <v>1460</v>
+        <v>1451</v>
       </c>
       <c r="D17" s="35" t="s">
-        <v>1460</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -14557,10 +14557,10 @@
         <v>1199</v>
       </c>
       <c r="B18" s="35" t="s">
-        <v>1460</v>
+        <v>1451</v>
       </c>
       <c r="D18" s="35" t="s">
-        <v>1460</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -14568,10 +14568,10 @@
         <v>1200</v>
       </c>
       <c r="B19" s="36" t="s">
-        <v>1466</v>
+        <v>1457</v>
       </c>
       <c r="C19" s="36" t="s">
-        <v>1467</v>
+        <v>1458</v>
       </c>
       <c r="D19" s="36"/>
     </row>
@@ -14580,10 +14580,10 @@
         <v>1201</v>
       </c>
       <c r="B20" s="36" t="s">
-        <v>1468</v>
+        <v>1459</v>
       </c>
       <c r="C20" s="36" t="s">
-        <v>1469</v>
+        <v>1460</v>
       </c>
       <c r="D20" s="36"/>
     </row>
@@ -14592,10 +14592,10 @@
         <v>1202</v>
       </c>
       <c r="B21" s="35" t="s">
-        <v>1470</v>
+        <v>1461</v>
       </c>
       <c r="C21" s="35" t="s">
-        <v>1471</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -14603,10 +14603,10 @@
         <v>1203</v>
       </c>
       <c r="B22" s="35" t="s">
-        <v>1472</v>
+        <v>1463</v>
       </c>
       <c r="C22" s="35" t="s">
-        <v>1473</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -14614,10 +14614,10 @@
         <v>1204</v>
       </c>
       <c r="B23" s="35" t="s">
-        <v>1474</v>
+        <v>1465</v>
       </c>
       <c r="C23" s="35" t="s">
-        <v>1475</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -14625,10 +14625,10 @@
         <v>1205</v>
       </c>
       <c r="B24" s="36" t="s">
-        <v>1476</v>
+        <v>1467</v>
       </c>
       <c r="C24" s="36" t="s">
-        <v>1477</v>
+        <v>1468</v>
       </c>
       <c r="D24" s="36"/>
     </row>
@@ -14637,10 +14637,10 @@
         <v>1206</v>
       </c>
       <c r="B25" s="36" t="s">
-        <v>1478</v>
+        <v>1469</v>
       </c>
       <c r="C25" s="36" t="s">
-        <v>1479</v>
+        <v>1470</v>
       </c>
       <c r="D25" s="36"/>
     </row>
@@ -14649,10 +14649,10 @@
         <v>1207</v>
       </c>
       <c r="B26" s="36" t="s">
-        <v>1480</v>
+        <v>1471</v>
       </c>
       <c r="C26" s="36" t="s">
-        <v>1481</v>
+        <v>1472</v>
       </c>
       <c r="D26" s="36"/>
     </row>
@@ -14661,10 +14661,10 @@
         <v>1208</v>
       </c>
       <c r="B27" s="36" t="s">
-        <v>1482</v>
+        <v>1473</v>
       </c>
       <c r="C27" s="36" t="s">
-        <v>1483</v>
+        <v>1474</v>
       </c>
       <c r="D27" s="36"/>
     </row>
@@ -14673,10 +14673,10 @@
         <v>1209</v>
       </c>
       <c r="B28" s="36" t="s">
-        <v>1484</v>
+        <v>1475</v>
       </c>
       <c r="C28" s="36" t="s">
-        <v>1485</v>
+        <v>1476</v>
       </c>
       <c r="D28" s="36"/>
     </row>
@@ -14685,7 +14685,7 @@
         <v>1210</v>
       </c>
       <c r="B29" s="36" t="s">
-        <v>1486</v>
+        <v>1477</v>
       </c>
       <c r="C29" s="36"/>
       <c r="D29" s="36"/>
@@ -14695,7 +14695,7 @@
         <v>1211</v>
       </c>
       <c r="B30" s="35" t="s">
-        <v>1487</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="31" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -14703,10 +14703,10 @@
         <v>1212</v>
       </c>
       <c r="B31" s="35" t="s">
-        <v>1488</v>
+        <v>1479</v>
       </c>
       <c r="C31" s="35" t="s">
-        <v>1489</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -14714,10 +14714,10 @@
         <v>1213</v>
       </c>
       <c r="B32" s="36" t="s">
-        <v>1490</v>
+        <v>1481</v>
       </c>
       <c r="C32" s="36" t="s">
-        <v>1491</v>
+        <v>1482</v>
       </c>
       <c r="D32" s="36"/>
     </row>
@@ -14726,10 +14726,10 @@
         <v>1214</v>
       </c>
       <c r="B33" s="36" t="s">
-        <v>1492</v>
+        <v>1483</v>
       </c>
       <c r="C33" s="36" t="s">
-        <v>1493</v>
+        <v>1484</v>
       </c>
       <c r="D33" s="36"/>
     </row>
@@ -14738,10 +14738,10 @@
         <v>1215</v>
       </c>
       <c r="B34" s="36" t="s">
-        <v>1494</v>
+        <v>1485</v>
       </c>
       <c r="C34" s="36" t="s">
-        <v>1495</v>
+        <v>1486</v>
       </c>
       <c r="D34" s="36"/>
     </row>
@@ -14750,10 +14750,10 @@
         <v>1216</v>
       </c>
       <c r="B35" s="36" t="s">
-        <v>1496</v>
+        <v>1487</v>
       </c>
       <c r="C35" s="36" t="s">
-        <v>1497</v>
+        <v>1488</v>
       </c>
       <c r="D35" s="36"/>
     </row>
@@ -14762,10 +14762,10 @@
         <v>1217</v>
       </c>
       <c r="B36" s="35" t="s">
-        <v>1498</v>
+        <v>1489</v>
       </c>
       <c r="C36" s="35" t="s">
-        <v>1499</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="37" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -14773,10 +14773,10 @@
         <v>1218</v>
       </c>
       <c r="B37" s="35" t="s">
-        <v>1500</v>
+        <v>1491</v>
       </c>
       <c r="C37" s="35" t="s">
-        <v>1501</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -14784,10 +14784,10 @@
         <v>1219</v>
       </c>
       <c r="B38" s="36" t="s">
-        <v>1502</v>
+        <v>1493</v>
       </c>
       <c r="C38" s="36" t="s">
-        <v>1503</v>
+        <v>1494</v>
       </c>
       <c r="D38" s="36"/>
     </row>
@@ -14796,10 +14796,10 @@
         <v>1220</v>
       </c>
       <c r="B39" s="36" t="s">
-        <v>1504</v>
+        <v>1495</v>
       </c>
       <c r="C39" s="36" t="s">
-        <v>1505</v>
+        <v>1496</v>
       </c>
       <c r="D39" s="36"/>
     </row>
@@ -14808,10 +14808,10 @@
         <v>1221</v>
       </c>
       <c r="B40" s="36" t="s">
-        <v>1506</v>
+        <v>1497</v>
       </c>
       <c r="C40" s="36" t="s">
-        <v>1505</v>
+        <v>1496</v>
       </c>
       <c r="D40" s="36"/>
     </row>
@@ -14820,10 +14820,10 @@
         <v>1222</v>
       </c>
       <c r="B41" s="35" t="s">
-        <v>1507</v>
+        <v>1498</v>
       </c>
       <c r="C41" s="35" t="s">
-        <v>1508</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="42" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -14831,10 +14831,10 @@
         <v>1223</v>
       </c>
       <c r="B42" s="35" t="s">
-        <v>1509</v>
+        <v>1500</v>
       </c>
       <c r="C42" s="35" t="s">
-        <v>1510</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="43" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -14842,10 +14842,10 @@
         <v>1224</v>
       </c>
       <c r="B43" s="35" t="s">
-        <v>1511</v>
+        <v>1502</v>
       </c>
       <c r="C43" s="35" t="s">
-        <v>1512</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="44" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -14853,10 +14853,10 @@
         <v>1225</v>
       </c>
       <c r="B44" s="35" t="s">
-        <v>1513</v>
+        <v>1504</v>
       </c>
       <c r="C44" s="35" t="s">
-        <v>1514</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="45" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -14864,10 +14864,10 @@
         <v>1226</v>
       </c>
       <c r="B45" s="35" t="s">
-        <v>1515</v>
+        <v>1506</v>
       </c>
       <c r="C45" s="35" t="s">
-        <v>1516</v>
+        <v>1507</v>
       </c>
     </row>
     <row r="46" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -14875,7 +14875,7 @@
         <v>1227</v>
       </c>
       <c r="B46" s="35" t="s">
-        <v>1517</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="47" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -14883,10 +14883,10 @@
         <v>1246</v>
       </c>
       <c r="B47" s="35" t="s">
-        <v>1518</v>
+        <v>1509</v>
       </c>
       <c r="C47" s="35" t="s">
-        <v>1519</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="48" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -14894,10 +14894,10 @@
         <v>1228</v>
       </c>
       <c r="B48" s="35" t="s">
-        <v>1520</v>
+        <v>1511</v>
       </c>
       <c r="C48" s="35" t="s">
-        <v>1521</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -14905,10 +14905,10 @@
         <v>1229</v>
       </c>
       <c r="B49" s="36" t="s">
-        <v>1522</v>
+        <v>1513</v>
       </c>
       <c r="C49" s="36" t="s">
-        <v>1523</v>
+        <v>1514</v>
       </c>
       <c r="D49" s="36"/>
     </row>
@@ -14917,10 +14917,10 @@
         <v>1230</v>
       </c>
       <c r="B50" s="36" t="s">
-        <v>1524</v>
+        <v>1515</v>
       </c>
       <c r="C50" s="36" t="s">
-        <v>1525</v>
+        <v>1516</v>
       </c>
       <c r="D50" s="36"/>
     </row>
@@ -14929,10 +14929,10 @@
         <v>1231</v>
       </c>
       <c r="B51" s="36" t="s">
-        <v>1526</v>
+        <v>1517</v>
       </c>
       <c r="C51" s="36" t="s">
-        <v>1527</v>
+        <v>1518</v>
       </c>
       <c r="D51" s="36"/>
     </row>
@@ -14941,10 +14941,10 @@
         <v>1232</v>
       </c>
       <c r="B52" s="35" t="s">
-        <v>1528</v>
+        <v>1519</v>
       </c>
       <c r="C52" s="35" t="s">
-        <v>1529</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="53" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -14952,10 +14952,10 @@
         <v>1233</v>
       </c>
       <c r="B53" s="35" t="s">
-        <v>1530</v>
+        <v>1521</v>
       </c>
       <c r="C53" s="35" t="s">
-        <v>1531</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="54" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -14963,21 +14963,21 @@
         <v>1234</v>
       </c>
       <c r="B54" s="35" t="s">
-        <v>1532</v>
+        <v>1523</v>
       </c>
       <c r="C54" s="35" t="s">
-        <v>1533</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="55" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="35" t="s">
-        <v>1534</v>
+        <v>1525</v>
       </c>
       <c r="B55" s="35" t="s">
-        <v>1535</v>
+        <v>1526</v>
       </c>
       <c r="C55" s="35" t="s">
-        <v>1536</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="56" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -14985,10 +14985,10 @@
         <v>1235</v>
       </c>
       <c r="B56" s="35" t="s">
-        <v>1537</v>
+        <v>1528</v>
       </c>
       <c r="C56" s="35" t="s">
-        <v>1538</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="57" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -14996,21 +14996,21 @@
         <v>1247</v>
       </c>
       <c r="B57" s="35" t="s">
-        <v>1539</v>
+        <v>1530</v>
       </c>
       <c r="C57" s="35" t="s">
-        <v>1540</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="58" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="35" t="s">
-        <v>1541</v>
+        <v>1532</v>
       </c>
       <c r="B58" s="35" t="s">
-        <v>1542</v>
+        <v>1533</v>
       </c>
       <c r="C58" s="35" t="s">
-        <v>1543</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="59" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -15018,10 +15018,10 @@
         <v>1236</v>
       </c>
       <c r="B59" s="35" t="s">
-        <v>1544</v>
+        <v>1535</v>
       </c>
       <c r="C59" s="35" t="s">
-        <v>1545</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="60" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -15029,10 +15029,10 @@
         <v>1238</v>
       </c>
       <c r="B60" s="35" t="s">
-        <v>1546</v>
+        <v>1537</v>
       </c>
       <c r="C60" s="35" t="s">
-        <v>1547</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="61" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -15040,10 +15040,10 @@
         <v>1239</v>
       </c>
       <c r="B61" s="35" t="s">
-        <v>1548</v>
+        <v>1539</v>
       </c>
       <c r="C61" s="35" t="s">
-        <v>1549</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="62" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -15051,10 +15051,10 @@
         <v>1237</v>
       </c>
       <c r="B62" s="35" t="s">
-        <v>1550</v>
+        <v>1541</v>
       </c>
       <c r="C62" s="35" t="s">
-        <v>1551</v>
+        <v>1542</v>
       </c>
     </row>
     <row r="63" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -15062,10 +15062,10 @@
         <v>1240</v>
       </c>
       <c r="B63" s="35" t="s">
-        <v>1552</v>
+        <v>1543</v>
       </c>
       <c r="C63" s="35" t="s">
-        <v>1553</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="64" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -15073,10 +15073,10 @@
         <v>1241</v>
       </c>
       <c r="B64" s="35" t="s">
-        <v>1554</v>
+        <v>1545</v>
       </c>
       <c r="C64" s="35" t="s">
-        <v>1555</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="65" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -15084,10 +15084,10 @@
         <v>1242</v>
       </c>
       <c r="B65" s="35" t="s">
-        <v>1556</v>
+        <v>1547</v>
       </c>
       <c r="C65" s="35" t="s">
-        <v>1557</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="66" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -15095,10 +15095,10 @@
         <v>1243</v>
       </c>
       <c r="B66" s="35" t="s">
-        <v>1558</v>
+        <v>1549</v>
       </c>
       <c r="C66" s="35" t="s">
-        <v>1559</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="67" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -15106,10 +15106,10 @@
         <v>1244</v>
       </c>
       <c r="B67" s="35" t="s">
-        <v>1560</v>
+        <v>1551</v>
       </c>
       <c r="C67" s="35" t="s">
-        <v>1561</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="68" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -15117,10 +15117,10 @@
         <v>1245</v>
       </c>
       <c r="B68" s="35" t="s">
-        <v>1562</v>
+        <v>1553</v>
       </c>
       <c r="C68" s="35" t="s">
-        <v>1563</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -15128,10 +15128,10 @@
         <v>1188</v>
       </c>
       <c r="B69" s="36" t="s">
-        <v>1564</v>
+        <v>1555</v>
       </c>
       <c r="C69" s="36" t="s">
-        <v>1565</v>
+        <v>1556</v>
       </c>
       <c r="D69" s="36"/>
     </row>
@@ -15140,10 +15140,10 @@
         <v>1189</v>
       </c>
       <c r="B70" s="36" t="s">
-        <v>1566</v>
+        <v>1557</v>
       </c>
       <c r="C70" s="36" t="s">
-        <v>1567</v>
+        <v>1558</v>
       </c>
       <c r="D70" s="36"/>
     </row>
@@ -15152,10 +15152,10 @@
         <v>1190</v>
       </c>
       <c r="B71" s="36" t="s">
-        <v>1568</v>
+        <v>1559</v>
       </c>
       <c r="C71" s="36" t="s">
-        <v>1569</v>
+        <v>1560</v>
       </c>
       <c r="D71" s="36"/>
     </row>
@@ -15164,10 +15164,10 @@
         <v>1191</v>
       </c>
       <c r="B72" s="36" t="s">
-        <v>1570</v>
+        <v>1561</v>
       </c>
       <c r="C72" s="36" t="s">
-        <v>1571</v>
+        <v>1562</v>
       </c>
       <c r="D72" s="36"/>
     </row>
@@ -15176,10 +15176,10 @@
         <v>1192</v>
       </c>
       <c r="B73" s="36" t="s">
-        <v>1572</v>
+        <v>1563</v>
       </c>
       <c r="C73" s="36" t="s">
-        <v>1573</v>
+        <v>1564</v>
       </c>
       <c r="D73" s="36"/>
     </row>
@@ -15188,10 +15188,10 @@
         <v>1193</v>
       </c>
       <c r="B74" s="36" t="s">
-        <v>1574</v>
+        <v>1565</v>
       </c>
       <c r="C74" s="36" t="s">
-        <v>1575</v>
+        <v>1566</v>
       </c>
       <c r="D74" s="36"/>
     </row>
@@ -15247,7 +15247,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>1454</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -15305,7 +15305,7 @@
         <v>30</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>1599</v>
+        <v>1590</v>
       </c>
       <c r="C12" s="25" t="s">
         <v>775</v>
@@ -17535,7 +17535,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>1454</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -17589,7 +17589,7 @@
         <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>1599</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -17682,74 +17682,74 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>1403</v>
+        <v>1401</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>1410</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>1404</v>
+        <v>1402</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>1412</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>1405</v>
+        <v>1403</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>1411</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>1406</v>
+        <v>1404</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>1409</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>1407</v>
+        <v>1405</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>1413</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>1408</v>
+        <v>1406</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>1415</v>
+        <v>1413</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>1418</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>1416</v>
+        <v>1414</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>1419</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>1417</v>
+        <v>1415</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>1420</v>
+        <v>1418</v>
       </c>
     </row>
   </sheetData>

</xml_diff>